<commit_message>
Added bonus to dialogue
</commit_message>
<xml_diff>
--- a/db/scenes.xlsx
+++ b/db/scenes.xlsx
@@ -5,14 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Scenes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TileSets" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Objects" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Containers" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Inventory" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -195,60 +194,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cannot search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mushroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A large, flat mushroom. Would be delicious grilled.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GoldCash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A few gleaming gold coins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BluePotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enchantment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A murky blue liquid. It bubbles slightly when shaken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GreenPotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A clear green liquid. Smoke rises from the top.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BlueWand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GreenWand</t>
   </si>
 </sst>
 </file>
@@ -691,7 +636,7 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -839,111 +784,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>